<commit_message>
LaTeX - Using actual AVG function
</commit_message>
<xml_diff>
--- a/Data/performance.xlsx
+++ b/Data/performance.xlsx
@@ -4075,7 +4075,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4420,19 +4420,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
-      <selection activeCell="K102" sqref="K102"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="N96" sqref="N96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.85546875" customWidth="1"/>
     <col min="2" max="3" width="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="5.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="4" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="13" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.85546875" customWidth="1"/>
+    <col min="12" max="13" width="5.42578125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="6" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="6.42578125" bestFit="1" customWidth="1"/>
     <col min="17" max="18" width="5.42578125" bestFit="1" customWidth="1"/>
@@ -13049,115 +13050,115 @@
     </row>
     <row r="102" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A102">
-        <f>AVERAGEA(A1:A100)</f>
+        <f>AVERAGE(A1:A100)</f>
         <v>155.19999999999999</v>
       </c>
       <c r="B102">
-        <f>AVERAGEA(B1:B100)</f>
+        <f>AVERAGE(B1:B100)</f>
         <v>35.92</v>
       </c>
       <c r="C102">
-        <f>AVERAGEA(C1:C100)</f>
+        <f>AVERAGE(C1:C100)</f>
         <v>37.880000000000003</v>
       </c>
       <c r="D102">
-        <f>AVERAGEA(D1:D100)</f>
+        <f>AVERAGE(D1:D100)</f>
         <v>1.7300000000000013E-3</v>
       </c>
       <c r="F102">
-        <f>AVERAGEA(F1:F100)</f>
-        <v>723.71</v>
+        <f>AVERAGE(F1:F100)</f>
+        <v>738.4795918367347</v>
       </c>
       <c r="G102">
-        <f>AVERAGEA(G1:G100)</f>
+        <f>AVERAGE(G1:G100)</f>
         <v>212.61</v>
       </c>
       <c r="H102">
-        <f>AVERAGEA(H1:H100)</f>
+        <f>AVERAGE(H1:H100)</f>
         <v>157.32</v>
       </c>
       <c r="I102">
-        <f>AVERAGEA(I1:I100)</f>
+        <f>AVERAGE(I1:I100)</f>
         <v>5.6100000000000039E-3</v>
       </c>
-      <c r="K102">
-        <f>AVERAGEA(K1:K100)</f>
-        <v>0</v>
+      <c r="K102" s="1" t="e">
+        <f>AVERAGE(K1:K100)</f>
+        <v>#DIV/0!</v>
       </c>
       <c r="L102">
-        <f>AVERAGEA(L1:L100)</f>
-        <v>362.53</v>
+        <f>AVERAGE(L1:L100)</f>
+        <v>575.44444444444446</v>
       </c>
       <c r="M102">
-        <f>AVERAGEA(M1:M100)</f>
-        <v>353.04</v>
+        <f>AVERAGE(M1:M100)</f>
+        <v>470.72</v>
       </c>
       <c r="N102">
-        <f>AVERAGEA(N1:N100)</f>
+        <f>AVERAGE(N1:N100)</f>
         <v>1.846999999999999E-2</v>
       </c>
-      <c r="P102">
-        <f>AVERAGEA(P1:P100)</f>
-        <v>0</v>
+      <c r="P102" t="e">
+        <f>AVERAGE(P1:P100)</f>
+        <v>#DIV/0!</v>
       </c>
       <c r="Q102">
-        <f>AVERAGEA(Q1:Q100)</f>
-        <v>26.19</v>
+        <f>AVERAGE(Q1:Q100)</f>
+        <v>327.375</v>
       </c>
       <c r="R102">
-        <f>AVERAGEA(R1:R100)</f>
-        <v>99.46</v>
+        <f>AVERAGE(R1:R100)</f>
+        <v>497.3</v>
       </c>
       <c r="S102">
-        <f>AVERAGEA(S1:S100)</f>
+        <f>AVERAGE(S1:S100)</f>
         <v>6.5629999999999994E-2</v>
       </c>
-      <c r="U102">
-        <f>AVERAGEA(U1:U100)</f>
-        <v>0</v>
+      <c r="U102" t="e">
+        <f>AVERAGE(U1:U100)</f>
+        <v>#DIV/0!</v>
       </c>
       <c r="V102">
-        <f>AVERAGEA(V1:V100)</f>
-        <v>9.4499999999999993</v>
+        <f>AVERAGE(V1:V100)</f>
+        <v>472.5</v>
       </c>
       <c r="W102">
-        <f>AVERAGEA(W1:W100)</f>
-        <v>19.84</v>
+        <f>AVERAGE(W1:W100)</f>
+        <v>396.8</v>
       </c>
       <c r="X102">
-        <f>AVERAGEA(X1:X100)</f>
+        <f>AVERAGE(X1:X100)</f>
         <v>0.37853999999999999</v>
       </c>
-      <c r="Z102">
-        <f>AVERAGEA(Z1:Z100)</f>
-        <v>0</v>
-      </c>
-      <c r="AA102">
-        <f>AVERAGEA(AA1:AA100)</f>
-        <v>0</v>
-      </c>
-      <c r="AB102">
-        <f>AVERAGEA(AB1:AB100)</f>
-        <v>0</v>
+      <c r="Z102" t="e">
+        <f>AVERAGE(Z1:Z100)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AA102" t="e">
+        <f>AVERAGE(AA1:AA100)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB102" t="e">
+        <f>AVERAGE(AB1:AB100)</f>
+        <v>#DIV/0!</v>
       </c>
       <c r="AC102">
-        <f>AVERAGEA(AC1:AC100)</f>
+        <f>AVERAGE(AC1:AC100)</f>
         <v>1.5292099999999997</v>
       </c>
-      <c r="AE102">
-        <f>AVERAGEA(AE1:AE100)</f>
-        <v>0</v>
+      <c r="AE102" t="e">
+        <f>AVERAGE(AE1:AE100)</f>
+        <v>#DIV/0!</v>
       </c>
       <c r="AF102">
-        <f>AVERAGEA(AF1:AF100)</f>
-        <v>0.93</v>
+        <f>AVERAGE(AF1:AF100)</f>
+        <v>93</v>
       </c>
       <c r="AG102">
-        <f>AVERAGEA(AG1:AG100)</f>
-        <v>8.68</v>
+        <f>AVERAGE(AG1:AG100)</f>
+        <v>868</v>
       </c>
       <c r="AH102">
-        <f>AVERAGEA(AH1:AH100)</f>
+        <f>AVERAGE(AH1:AH100)</f>
         <v>6.7504100000000014</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Data - Added standard deviation to the performance excel sheet
</commit_message>
<xml_diff>
--- a/Data/performance.xlsx
+++ b/Data/performance.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17927"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18067"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -107,6 +107,10 @@
 </connections>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
@@ -158,31 +162,31 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="city_25" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="city_1000" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="city_500" connectionId="7" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="city_10" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="city_250" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="city_100" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="city_50" connectionId="6" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="city_25" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="city_10" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -482,10 +486,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AH102"/>
+  <dimension ref="A1:AH206"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="W105" sqref="W105"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F206" sqref="F206"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9235,6 +9239,3032 @@
         <v>6.7504100000000014</v>
       </c>
     </row>
+    <row r="105" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A105">
+        <f>($A1-$A$102)^2</f>
+        <v>231.03999999999965</v>
+      </c>
+      <c r="F105">
+        <f>($F1-$F$102)^2</f>
+        <v>24579.968399999991</v>
+      </c>
+      <c r="K105">
+        <f>($K1-$K$102)^2</f>
+        <v>358932.79210000014</v>
+      </c>
+      <c r="P105">
+        <f>($P1-$P$102)^2</f>
+        <v>885763.32249999931</v>
+      </c>
+      <c r="U105">
+        <f>($U1-$U$102)^2</f>
+        <v>277549.84890000185</v>
+      </c>
+      <c r="Z105">
+        <f>($Z1-$Z$102)^2</f>
+        <v>237204662.10250035</v>
+      </c>
+      <c r="AE105">
+        <f>($AE1-$AE$102)^2</f>
+        <v>143664370090.48895</v>
+      </c>
+    </row>
+    <row r="106" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A106">
+        <f t="shared" ref="A106:A169" si="7">($A2-$A$102)^2</f>
+        <v>1584.0400000000009</v>
+      </c>
+      <c r="F106">
+        <f t="shared" ref="F106:F169" si="8">($F2-$F$102)^2</f>
+        <v>138.76839999999936</v>
+      </c>
+      <c r="K106">
+        <f t="shared" ref="K106:K169" si="9">($K2-$K$102)^2</f>
+        <v>152794.99209999989</v>
+      </c>
+      <c r="P106">
+        <f t="shared" ref="P106:P169" si="10">($P2-$P$102)^2</f>
+        <v>145275.32249999972</v>
+      </c>
+      <c r="U106">
+        <f t="shared" ref="U106:U169" si="11">($U2-$U$102)^2</f>
+        <v>135998278.94890004</v>
+      </c>
+      <c r="Z106">
+        <f t="shared" ref="Z106:Z169" si="12">($Z2-$Z$102)^2</f>
+        <v>299167182.60250038</v>
+      </c>
+      <c r="AE106">
+        <f t="shared" ref="AE106:AE169" si="13">($AE2-$AE$102)^2</f>
+        <v>13282062319.708918</v>
+      </c>
+    </row>
+    <row r="107" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A107">
+        <f t="shared" si="7"/>
+        <v>1584.0400000000009</v>
+      </c>
+      <c r="F107">
+        <f t="shared" si="8"/>
+        <v>5072.288400000004</v>
+      </c>
+      <c r="K107">
+        <f t="shared" si="9"/>
+        <v>41660.892100000056</v>
+      </c>
+      <c r="P107">
+        <f t="shared" si="10"/>
+        <v>659587.62249999936</v>
+      </c>
+      <c r="U107">
+        <f t="shared" si="11"/>
+        <v>108260487.32890004</v>
+      </c>
+      <c r="Z107">
+        <f t="shared" si="12"/>
+        <v>101756647.50250024</v>
+      </c>
+      <c r="AE107">
+        <f t="shared" si="13"/>
+        <v>67026709049.328865</v>
+      </c>
+    </row>
+    <row r="108" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A108">
+        <f t="shared" si="7"/>
+        <v>316.84000000000043</v>
+      </c>
+      <c r="F108">
+        <f t="shared" si="8"/>
+        <v>12593.328400000006</v>
+      </c>
+      <c r="K108">
+        <f t="shared" si="9"/>
+        <v>75685.512100000065</v>
+      </c>
+      <c r="P108">
+        <f t="shared" si="10"/>
+        <v>12822486.722500002</v>
+      </c>
+      <c r="U108">
+        <f t="shared" si="11"/>
+        <v>285502864.04890007</v>
+      </c>
+      <c r="Z108">
+        <f t="shared" si="12"/>
+        <v>7915918915.1025019</v>
+      </c>
+      <c r="AE108">
+        <f t="shared" si="13"/>
+        <v>6578642303.9689121</v>
+      </c>
+    </row>
+    <row r="109" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A109">
+        <f t="shared" si="7"/>
+        <v>1459.2399999999991</v>
+      </c>
+      <c r="F109">
+        <f t="shared" si="8"/>
+        <v>10654.368400000005</v>
+      </c>
+      <c r="K109">
+        <f t="shared" si="9"/>
+        <v>108972.61210000009</v>
+      </c>
+      <c r="P109">
+        <f t="shared" si="10"/>
+        <v>4883437.0225000018</v>
+      </c>
+      <c r="U109">
+        <f t="shared" si="11"/>
+        <v>128282126.86889996</v>
+      </c>
+      <c r="Z109">
+        <f t="shared" si="12"/>
+        <v>82599923.402500212</v>
+      </c>
+      <c r="AE109">
+        <f t="shared" si="13"/>
+        <v>613165063.10889626</v>
+      </c>
+    </row>
+    <row r="110" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A110">
+        <f t="shared" si="7"/>
+        <v>2134.4399999999991</v>
+      </c>
+      <c r="F110">
+        <f t="shared" si="8"/>
+        <v>16584.288399999994</v>
+      </c>
+      <c r="K110">
+        <f t="shared" si="9"/>
+        <v>269475.19210000016</v>
+      </c>
+      <c r="P110">
+        <f t="shared" si="10"/>
+        <v>1223567.8224999993</v>
+      </c>
+      <c r="U110">
+        <f t="shared" si="11"/>
+        <v>27281504.848899983</v>
+      </c>
+      <c r="Z110">
+        <f t="shared" si="12"/>
+        <v>455163023.70249951</v>
+      </c>
+      <c r="AE110">
+        <f t="shared" si="13"/>
+        <v>50358425350.648933</v>
+      </c>
+    </row>
+    <row r="111" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A111">
+        <f t="shared" si="7"/>
+        <v>1383.8399999999992</v>
+      </c>
+      <c r="F111">
+        <f t="shared" si="8"/>
+        <v>5361.1684000000041</v>
+      </c>
+      <c r="K111">
+        <f t="shared" si="9"/>
+        <v>94931.772100000075</v>
+      </c>
+      <c r="P111">
+        <f t="shared" si="10"/>
+        <v>2013135.3225000009</v>
+      </c>
+      <c r="U111">
+        <f t="shared" si="11"/>
+        <v>713272929.4088999</v>
+      </c>
+      <c r="Z111">
+        <f t="shared" si="12"/>
+        <v>535850737.40250051</v>
+      </c>
+      <c r="AE111">
+        <f t="shared" si="13"/>
+        <v>15684514063.108919</v>
+      </c>
+    </row>
+    <row r="112" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A112">
+        <f t="shared" si="7"/>
+        <v>2580.6400000000012</v>
+      </c>
+      <c r="F112">
+        <f t="shared" si="8"/>
+        <v>15931.488400000007</v>
+      </c>
+      <c r="K112">
+        <f t="shared" si="9"/>
+        <v>81858.932100000078</v>
+      </c>
+      <c r="P112">
+        <f t="shared" si="10"/>
+        <v>3139452.4225000013</v>
+      </c>
+      <c r="U112">
+        <f t="shared" si="11"/>
+        <v>145367149.64890003</v>
+      </c>
+      <c r="Z112">
+        <f t="shared" si="12"/>
+        <v>319210035.60250044</v>
+      </c>
+      <c r="AE112">
+        <f t="shared" si="13"/>
+        <v>43041796763.128868</v>
+      </c>
+    </row>
+    <row r="113" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A113">
+        <f t="shared" si="7"/>
+        <v>27.039999999999882</v>
+      </c>
+      <c r="F113">
+        <f t="shared" si="8"/>
+        <v>3389.5684000000033</v>
+      </c>
+      <c r="K113">
+        <f t="shared" si="9"/>
+        <v>883806.81210000021</v>
+      </c>
+      <c r="P113">
+        <f t="shared" si="10"/>
+        <v>612854.12250000052</v>
+      </c>
+      <c r="U113">
+        <f t="shared" si="11"/>
+        <v>43018250.968900025</v>
+      </c>
+      <c r="Z113">
+        <f t="shared" si="12"/>
+        <v>362999661.50249958</v>
+      </c>
+      <c r="AE113">
+        <f t="shared" si="13"/>
+        <v>17913635457.74892</v>
+      </c>
+    </row>
+    <row r="114" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A114">
+        <f t="shared" si="7"/>
+        <v>912.03999999999928</v>
+      </c>
+      <c r="F114">
+        <f t="shared" si="8"/>
+        <v>13872.128399999994</v>
+      </c>
+      <c r="K114">
+        <f t="shared" si="9"/>
+        <v>524016.73209999979</v>
+      </c>
+      <c r="P114">
+        <f t="shared" si="10"/>
+        <v>6629852.5225000018</v>
+      </c>
+      <c r="U114">
+        <f t="shared" si="11"/>
+        <v>13229005.608899986</v>
+      </c>
+      <c r="Z114">
+        <f t="shared" si="12"/>
+        <v>3195929209.5024986</v>
+      </c>
+      <c r="AE114">
+        <f t="shared" si="13"/>
+        <v>11924677128.028883</v>
+      </c>
+    </row>
+    <row r="115" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A115">
+        <f t="shared" si="7"/>
+        <v>96.040000000000219</v>
+      </c>
+      <c r="F115">
+        <f t="shared" si="8"/>
+        <v>40489.488400000009</v>
+      </c>
+      <c r="K115">
+        <f t="shared" si="9"/>
+        <v>89335.232099999921</v>
+      </c>
+      <c r="P115">
+        <f t="shared" si="10"/>
+        <v>104425.92249999977</v>
+      </c>
+      <c r="U115">
+        <f t="shared" si="11"/>
+        <v>4227835.0688999929</v>
+      </c>
+      <c r="Z115">
+        <f t="shared" si="12"/>
+        <v>3527237429.3024988</v>
+      </c>
+      <c r="AE115">
+        <f t="shared" si="13"/>
+        <v>15177458922.048918</v>
+      </c>
+    </row>
+    <row r="116" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A116">
+        <f t="shared" si="7"/>
+        <v>190.44000000000031</v>
+      </c>
+      <c r="F116">
+        <f t="shared" si="8"/>
+        <v>8423.5683999999947</v>
+      </c>
+      <c r="K116">
+        <f t="shared" si="9"/>
+        <v>866965.83210000023</v>
+      </c>
+      <c r="P116">
+        <f t="shared" si="10"/>
+        <v>11938061.522499997</v>
+      </c>
+      <c r="U116">
+        <f t="shared" si="11"/>
+        <v>246055929.26889995</v>
+      </c>
+      <c r="Z116">
+        <f t="shared" si="12"/>
+        <v>646458592.80249941</v>
+      </c>
+      <c r="AE116">
+        <f t="shared" si="13"/>
+        <v>16022648.008900596</v>
+      </c>
+    </row>
+    <row r="117" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A117">
+        <f t="shared" si="7"/>
+        <v>7.8400000000000638</v>
+      </c>
+      <c r="F117">
+        <f t="shared" si="8"/>
+        <v>42115.248400000011</v>
+      </c>
+      <c r="K117">
+        <f t="shared" si="9"/>
+        <v>15903.732100000032</v>
+      </c>
+      <c r="P117">
+        <f t="shared" si="10"/>
+        <v>2387488.522499999</v>
+      </c>
+      <c r="U117">
+        <f t="shared" si="11"/>
+        <v>316777.60890000197</v>
+      </c>
+      <c r="Z117">
+        <f t="shared" si="12"/>
+        <v>91155711.002499774</v>
+      </c>
+      <c r="AE117">
+        <f t="shared" si="13"/>
+        <v>2163102894.0888929</v>
+      </c>
+    </row>
+    <row r="118" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A118">
+        <f t="shared" si="7"/>
+        <v>1383.8399999999992</v>
+      </c>
+      <c r="F118">
+        <f t="shared" si="8"/>
+        <v>10.368400000000175</v>
+      </c>
+      <c r="K118">
+        <f t="shared" si="9"/>
+        <v>29890.952099999955</v>
+      </c>
+      <c r="P118">
+        <f t="shared" si="10"/>
+        <v>1564625.7225000008</v>
+      </c>
+      <c r="U118">
+        <f t="shared" si="11"/>
+        <v>222511817.24890006</v>
+      </c>
+      <c r="Z118">
+        <f t="shared" si="12"/>
+        <v>2419700371.2025013</v>
+      </c>
+      <c r="AE118">
+        <f t="shared" si="13"/>
+        <v>6496816204.0089121</v>
+      </c>
+    </row>
+    <row r="119" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A119">
+        <f t="shared" si="7"/>
+        <v>492.83999999999952</v>
+      </c>
+      <c r="F119">
+        <f t="shared" si="8"/>
+        <v>86306.688399999985</v>
+      </c>
+      <c r="K119">
+        <f t="shared" si="9"/>
+        <v>3955.1520999999839</v>
+      </c>
+      <c r="P119">
+        <f t="shared" si="10"/>
+        <v>6279284.222500002</v>
+      </c>
+      <c r="U119">
+        <f t="shared" si="11"/>
+        <v>360575664.76890004</v>
+      </c>
+      <c r="Z119">
+        <f t="shared" si="12"/>
+        <v>2499755006.0024986</v>
+      </c>
+      <c r="AE119">
+        <f t="shared" si="13"/>
+        <v>5850082190.7889118</v>
+      </c>
+    </row>
+    <row r="120" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A120">
+        <f t="shared" si="7"/>
+        <v>1310.4399999999991</v>
+      </c>
+      <c r="F120">
+        <f t="shared" si="8"/>
+        <v>9956.0483999999942</v>
+      </c>
+      <c r="K120">
+        <f t="shared" si="9"/>
+        <v>98526.932099999918</v>
+      </c>
+      <c r="P120">
+        <f t="shared" si="10"/>
+        <v>5509113.1224999987</v>
+      </c>
+      <c r="U120">
+        <f t="shared" si="11"/>
+        <v>280869779.08889997</v>
+      </c>
+      <c r="Z120">
+        <f t="shared" si="12"/>
+        <v>419084359.4024995</v>
+      </c>
+      <c r="AE120">
+        <f t="shared" si="13"/>
+        <v>5886239198.5489111</v>
+      </c>
+    </row>
+    <row r="121" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A121">
+        <f t="shared" si="7"/>
+        <v>10.239999999999927</v>
+      </c>
+      <c r="F121">
+        <f t="shared" si="8"/>
+        <v>16073.168399999993</v>
+      </c>
+      <c r="K121">
+        <f t="shared" si="9"/>
+        <v>47912.832099999941</v>
+      </c>
+      <c r="P121">
+        <f t="shared" si="10"/>
+        <v>806134.62250000064</v>
+      </c>
+      <c r="U121">
+        <f t="shared" si="11"/>
+        <v>644356086.58889997</v>
+      </c>
+      <c r="Z121">
+        <f t="shared" si="12"/>
+        <v>473430146.40250051</v>
+      </c>
+      <c r="AE121">
+        <f t="shared" si="13"/>
+        <v>4885893966.6888895</v>
+      </c>
+    </row>
+    <row r="122" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A122">
+        <f t="shared" si="7"/>
+        <v>84.639999999999787</v>
+      </c>
+      <c r="F122">
+        <f t="shared" si="8"/>
+        <v>5152.3683999999957</v>
+      </c>
+      <c r="K122">
+        <f t="shared" si="9"/>
+        <v>1461415.0320999997</v>
+      </c>
+      <c r="P122">
+        <f t="shared" si="10"/>
+        <v>707533.32249999943</v>
+      </c>
+      <c r="U122">
+        <f t="shared" si="11"/>
+        <v>120103407.08889996</v>
+      </c>
+      <c r="Z122">
+        <f t="shared" si="12"/>
+        <v>3226529686.5024986</v>
+      </c>
+      <c r="AE122">
+        <f t="shared" si="13"/>
+        <v>49561369683.868935</v>
+      </c>
+    </row>
+    <row r="123" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A123">
+        <f t="shared" si="7"/>
+        <v>2134.4399999999991</v>
+      </c>
+      <c r="F123">
+        <f t="shared" si="8"/>
+        <v>6049.7283999999954</v>
+      </c>
+      <c r="K123">
+        <f t="shared" si="9"/>
+        <v>75564.512099999934</v>
+      </c>
+      <c r="P123">
+        <f t="shared" si="10"/>
+        <v>127556.12249999974</v>
+      </c>
+      <c r="U123">
+        <f t="shared" si="11"/>
+        <v>8644599.6288999896</v>
+      </c>
+      <c r="Z123">
+        <f t="shared" si="12"/>
+        <v>1708379689.5024991</v>
+      </c>
+      <c r="AE123">
+        <f t="shared" si="13"/>
+        <v>136120538466.32884</v>
+      </c>
+    </row>
+    <row r="124" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A124">
+        <f t="shared" si="7"/>
+        <v>2580.6400000000012</v>
+      </c>
+      <c r="F124">
+        <f t="shared" si="8"/>
+        <v>10359.168399999995</v>
+      </c>
+      <c r="K124">
+        <f t="shared" si="9"/>
+        <v>217986.27209999989</v>
+      </c>
+      <c r="P124">
+        <f t="shared" si="10"/>
+        <v>342400.52249999956</v>
+      </c>
+      <c r="U124">
+        <f t="shared" si="11"/>
+        <v>40528120.46889998</v>
+      </c>
+      <c r="Z124">
+        <f t="shared" si="12"/>
+        <v>1659873896.402499</v>
+      </c>
+      <c r="AE124">
+        <f t="shared" si="13"/>
+        <v>497431392.04889667</v>
+      </c>
+    </row>
+    <row r="125" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A125">
+        <f t="shared" si="7"/>
+        <v>331.23999999999961</v>
+      </c>
+      <c r="F125">
+        <f t="shared" si="8"/>
+        <v>2681.1683999999973</v>
+      </c>
+      <c r="K125">
+        <f t="shared" si="9"/>
+        <v>3493.9921000000149</v>
+      </c>
+      <c r="P125">
+        <f t="shared" si="10"/>
+        <v>200.22249999998971</v>
+      </c>
+      <c r="U125">
+        <f t="shared" si="11"/>
+        <v>40016125.188900024</v>
+      </c>
+      <c r="Z125">
+        <f t="shared" si="12"/>
+        <v>4285201436.1025014</v>
+      </c>
+      <c r="AE125">
+        <f t="shared" si="13"/>
+        <v>5829501160.3688889</v>
+      </c>
+    </row>
+    <row r="126" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A126">
+        <f t="shared" si="7"/>
+        <v>368.63999999999959</v>
+      </c>
+      <c r="F126">
+        <f t="shared" si="8"/>
+        <v>7.7283999999998487</v>
+      </c>
+      <c r="K126">
+        <f t="shared" si="9"/>
+        <v>18195.312099999966</v>
+      </c>
+      <c r="P126">
+        <f t="shared" si="10"/>
+        <v>1048883.2224999992</v>
+      </c>
+      <c r="U126">
+        <f t="shared" si="11"/>
+        <v>70439595.408900023</v>
+      </c>
+      <c r="Z126">
+        <f t="shared" si="12"/>
+        <v>201198621.80250034</v>
+      </c>
+      <c r="AE126">
+        <f t="shared" si="13"/>
+        <v>50488665412.048935</v>
+      </c>
+    </row>
+    <row r="127" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A127">
+        <f t="shared" si="7"/>
+        <v>3.9999999999995456E-2</v>
+      </c>
+      <c r="F127">
+        <f t="shared" si="8"/>
+        <v>2229.7284000000027</v>
+      </c>
+      <c r="K127">
+        <f t="shared" si="9"/>
+        <v>109633.83210000009</v>
+      </c>
+      <c r="P127">
+        <f t="shared" si="10"/>
+        <v>670515.32250000059</v>
+      </c>
+      <c r="U127">
+        <f t="shared" si="11"/>
+        <v>28720703.088899981</v>
+      </c>
+      <c r="Z127">
+        <f t="shared" si="12"/>
+        <v>138616479.60249972</v>
+      </c>
+      <c r="AE127">
+        <f t="shared" si="13"/>
+        <v>88607530107.828857</v>
+      </c>
+    </row>
+    <row r="128" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A128">
+        <f t="shared" si="7"/>
+        <v>125.43999999999974</v>
+      </c>
+      <c r="F128">
+        <f t="shared" si="8"/>
+        <v>34677.888400000011</v>
+      </c>
+      <c r="K128">
+        <f t="shared" si="9"/>
+        <v>1001780.7920999997</v>
+      </c>
+      <c r="P128">
+        <f t="shared" si="10"/>
+        <v>435798.0224999995</v>
+      </c>
+      <c r="U128">
+        <f t="shared" si="11"/>
+        <v>122925338.60889997</v>
+      </c>
+      <c r="Z128">
+        <f t="shared" si="12"/>
+        <v>159023449.20250028</v>
+      </c>
+      <c r="AE128">
+        <f t="shared" si="13"/>
+        <v>46919818452.628929</v>
+      </c>
+    </row>
+    <row r="129" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A129">
+        <f t="shared" si="7"/>
+        <v>519.84000000000049</v>
+      </c>
+      <c r="F129">
+        <f t="shared" si="8"/>
+        <v>30548.048399999989</v>
+      </c>
+      <c r="K129">
+        <f t="shared" si="9"/>
+        <v>206215.89210000011</v>
+      </c>
+      <c r="P129">
+        <f t="shared" si="10"/>
+        <v>511439.5224999995</v>
+      </c>
+      <c r="U129">
+        <f t="shared" si="11"/>
+        <v>11622440.088899989</v>
+      </c>
+      <c r="Z129">
+        <f t="shared" si="12"/>
+        <v>336702315.30250043</v>
+      </c>
+      <c r="AE129">
+        <f t="shared" si="13"/>
+        <v>8302276709.2489138</v>
+      </c>
+    </row>
+    <row r="130" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A130">
+        <f t="shared" si="7"/>
+        <v>38.439999999999856</v>
+      </c>
+      <c r="F130">
+        <f t="shared" si="8"/>
+        <v>21251.808399999991</v>
+      </c>
+      <c r="K130">
+        <f t="shared" si="9"/>
+        <v>43218.252099999947</v>
+      </c>
+      <c r="P130">
+        <f t="shared" si="10"/>
+        <v>3207143.7225000011</v>
+      </c>
+      <c r="U130">
+        <f t="shared" si="11"/>
+        <v>872038.46890000324</v>
+      </c>
+      <c r="Z130">
+        <f t="shared" si="12"/>
+        <v>726811944.30250061</v>
+      </c>
+      <c r="AE130">
+        <f t="shared" si="13"/>
+        <v>253874063193.08884</v>
+      </c>
+    </row>
+    <row r="131" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A131">
+        <f t="shared" si="7"/>
+        <v>262.43999999999966</v>
+      </c>
+      <c r="F131">
+        <f t="shared" si="8"/>
+        <v>10044.048400000005</v>
+      </c>
+      <c r="K131">
+        <f t="shared" si="9"/>
+        <v>1081.7520999999915</v>
+      </c>
+      <c r="P131">
+        <f t="shared" si="10"/>
+        <v>21602509.622500002</v>
+      </c>
+      <c r="U131">
+        <f t="shared" si="11"/>
+        <v>215908640.06890005</v>
+      </c>
+      <c r="Z131">
+        <f t="shared" si="12"/>
+        <v>117471998.40250026</v>
+      </c>
+      <c r="AE131">
+        <f t="shared" si="13"/>
+        <v>73888738204.528946</v>
+      </c>
+    </row>
+    <row r="132" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A132">
+        <f t="shared" si="7"/>
+        <v>449.43999999999954</v>
+      </c>
+      <c r="F132">
+        <f t="shared" si="8"/>
+        <v>189.88839999999925</v>
+      </c>
+      <c r="K132">
+        <f t="shared" si="9"/>
+        <v>164925.33210000012</v>
+      </c>
+      <c r="P132">
+        <f t="shared" si="10"/>
+        <v>1502708.2225000008</v>
+      </c>
+      <c r="U132">
+        <f t="shared" si="11"/>
+        <v>320296524.04890007</v>
+      </c>
+      <c r="Z132">
+        <f t="shared" si="12"/>
+        <v>564677.1025000175</v>
+      </c>
+      <c r="AE132">
+        <f t="shared" si="13"/>
+        <v>96465421320.768951</v>
+      </c>
+    </row>
+    <row r="133" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A133">
+        <f t="shared" si="7"/>
+        <v>615.04000000000053</v>
+      </c>
+      <c r="F133">
+        <f t="shared" si="8"/>
+        <v>13507.088400000006</v>
+      </c>
+      <c r="K133">
+        <f t="shared" si="9"/>
+        <v>131848.8721000001</v>
+      </c>
+      <c r="P133">
+        <f t="shared" si="10"/>
+        <v>290359.32250000042</v>
+      </c>
+      <c r="U133">
+        <f t="shared" si="11"/>
+        <v>79266436.048899963</v>
+      </c>
+      <c r="Z133">
+        <f t="shared" si="12"/>
+        <v>170813137.20249969</v>
+      </c>
+      <c r="AE133">
+        <f t="shared" si="13"/>
+        <v>140994369731.30884</v>
+      </c>
+    </row>
+    <row r="134" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A134">
+        <f t="shared" si="7"/>
+        <v>1747.2400000000009</v>
+      </c>
+      <c r="F134">
+        <f t="shared" si="8"/>
+        <v>45.968399999999633</v>
+      </c>
+      <c r="K134">
+        <f t="shared" si="9"/>
+        <v>116888.77209999991</v>
+      </c>
+      <c r="P134">
+        <f t="shared" si="10"/>
+        <v>6523682.2224999983</v>
+      </c>
+      <c r="U134">
+        <f t="shared" si="11"/>
+        <v>132614340.58890004</v>
+      </c>
+      <c r="Z134">
+        <f t="shared" si="12"/>
+        <v>1166048341.5025008</v>
+      </c>
+      <c r="AE134">
+        <f t="shared" si="13"/>
+        <v>25130546574.868877</v>
+      </c>
+    </row>
+    <row r="135" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A135">
+        <f t="shared" si="7"/>
+        <v>27.039999999999882</v>
+      </c>
+      <c r="F135">
+        <f t="shared" si="8"/>
+        <v>22566.048400000007</v>
+      </c>
+      <c r="K135">
+        <f t="shared" si="9"/>
+        <v>89934.01209999992</v>
+      </c>
+      <c r="P135">
+        <f t="shared" si="10"/>
+        <v>191100.12249999968</v>
+      </c>
+      <c r="U135">
+        <f t="shared" si="11"/>
+        <v>64013280.688900031</v>
+      </c>
+      <c r="Z135">
+        <f t="shared" si="12"/>
+        <v>7703677.802499935</v>
+      </c>
+      <c r="AE135">
+        <f t="shared" si="13"/>
+        <v>338679967311.10883</v>
+      </c>
+    </row>
+    <row r="136" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A136">
+        <f t="shared" si="7"/>
+        <v>1918.440000000001</v>
+      </c>
+      <c r="F136">
+        <f t="shared" si="8"/>
+        <v>2282.9283999999975</v>
+      </c>
+      <c r="K136">
+        <f t="shared" si="9"/>
+        <v>16355.852099999967</v>
+      </c>
+      <c r="P136">
+        <f t="shared" si="10"/>
+        <v>888966.12250000064</v>
+      </c>
+      <c r="U136">
+        <f t="shared" si="11"/>
+        <v>60034138.348899975</v>
+      </c>
+      <c r="Z136">
+        <f t="shared" si="12"/>
+        <v>1868448172.8024991</v>
+      </c>
+      <c r="AE136">
+        <f t="shared" si="13"/>
+        <v>52968640451.688866</v>
+      </c>
+    </row>
+    <row r="137" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A137">
+        <f t="shared" si="7"/>
+        <v>829.44000000000062</v>
+      </c>
+      <c r="F137">
+        <f t="shared" si="8"/>
+        <v>8241.0083999999952</v>
+      </c>
+      <c r="K137">
+        <f t="shared" si="9"/>
+        <v>3351.2520999999851</v>
+      </c>
+      <c r="P137">
+        <f t="shared" si="10"/>
+        <v>110124.42250000025</v>
+      </c>
+      <c r="U137">
+        <f t="shared" si="11"/>
+        <v>178859328.86890006</v>
+      </c>
+      <c r="Z137">
+        <f t="shared" si="12"/>
+        <v>1164962705.4024992</v>
+      </c>
+      <c r="AE137">
+        <f t="shared" si="13"/>
+        <v>31267494396.868874</v>
+      </c>
+    </row>
+    <row r="138" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A138">
+        <f t="shared" si="7"/>
+        <v>163.84000000000029</v>
+      </c>
+      <c r="F138">
+        <f t="shared" si="8"/>
+        <v>1103.5684000000017</v>
+      </c>
+      <c r="K138">
+        <f t="shared" si="9"/>
+        <v>29203.392099999957</v>
+      </c>
+      <c r="P138">
+        <f t="shared" si="10"/>
+        <v>7777684.3225000016</v>
+      </c>
+      <c r="U138">
+        <f t="shared" si="11"/>
+        <v>104717768.24889997</v>
+      </c>
+      <c r="Z138">
+        <f t="shared" si="12"/>
+        <v>13954333.802499913</v>
+      </c>
+      <c r="AE138">
+        <f t="shared" si="13"/>
+        <v>95203614693.68895</v>
+      </c>
+    </row>
+    <row r="139" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A139">
+        <f t="shared" si="7"/>
+        <v>1616.0399999999991</v>
+      </c>
+      <c r="F139">
+        <f t="shared" si="8"/>
+        <v>10.368400000000175</v>
+      </c>
+      <c r="K139">
+        <f t="shared" si="9"/>
+        <v>3955.1520999999839</v>
+      </c>
+      <c r="P139">
+        <f t="shared" si="10"/>
+        <v>7393776.7224999983</v>
+      </c>
+      <c r="U139">
+        <f t="shared" si="11"/>
+        <v>32362786.768900018</v>
+      </c>
+      <c r="Z139">
+        <f t="shared" si="12"/>
+        <v>5136795.6025000531</v>
+      </c>
+      <c r="AE139">
+        <f t="shared" si="13"/>
+        <v>55654136.428898886</v>
+      </c>
+    </row>
+    <row r="140" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A140">
+        <f t="shared" si="7"/>
+        <v>1310.4399999999991</v>
+      </c>
+      <c r="F140">
+        <f t="shared" si="8"/>
+        <v>740.92840000000149</v>
+      </c>
+      <c r="K140">
+        <f t="shared" si="9"/>
+        <v>99155.712099999917</v>
+      </c>
+      <c r="P140">
+        <f t="shared" si="10"/>
+        <v>4182638.5224999986</v>
+      </c>
+      <c r="U140">
+        <f t="shared" si="11"/>
+        <v>52806818.248900026</v>
+      </c>
+      <c r="Z140">
+        <f t="shared" si="12"/>
+        <v>1210869486.0024991</v>
+      </c>
+      <c r="AE140">
+        <f t="shared" si="13"/>
+        <v>96251854541.728943</v>
+      </c>
+    </row>
+    <row r="141" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A141">
+        <f t="shared" si="7"/>
+        <v>262.43999999999966</v>
+      </c>
+      <c r="F141">
+        <f t="shared" si="8"/>
+        <v>6435.248400000004</v>
+      </c>
+      <c r="K141">
+        <f t="shared" si="9"/>
+        <v>575914.03209999984</v>
+      </c>
+      <c r="P141">
+        <f t="shared" si="10"/>
+        <v>4423239.9224999985</v>
+      </c>
+      <c r="U141">
+        <f t="shared" si="11"/>
+        <v>280132859.60889995</v>
+      </c>
+      <c r="Z141">
+        <f t="shared" si="12"/>
+        <v>661592990.10250056</v>
+      </c>
+      <c r="AE141">
+        <f t="shared" si="13"/>
+        <v>60284082263.548866</v>
+      </c>
+    </row>
+    <row r="142" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A142">
+        <f t="shared" si="7"/>
+        <v>2043.0399999999991</v>
+      </c>
+      <c r="F142">
+        <f t="shared" si="8"/>
+        <v>8608.1283999999941</v>
+      </c>
+      <c r="K142">
+        <f t="shared" si="9"/>
+        <v>90534.792099999919</v>
+      </c>
+      <c r="P142">
+        <f t="shared" si="10"/>
+        <v>94156.922500000219</v>
+      </c>
+      <c r="U142">
+        <f t="shared" si="11"/>
+        <v>15200875.368900014</v>
+      </c>
+      <c r="Z142">
+        <f t="shared" si="12"/>
+        <v>4412885113.2024984</v>
+      </c>
+      <c r="AE142">
+        <f t="shared" si="13"/>
+        <v>66463845981.988937</v>
+      </c>
+    </row>
+    <row r="143" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A143">
+        <f t="shared" si="7"/>
+        <v>1211.0400000000009</v>
+      </c>
+      <c r="F143">
+        <f t="shared" si="8"/>
+        <v>11189.408399999995</v>
+      </c>
+      <c r="K143">
+        <f t="shared" si="9"/>
+        <v>65.772100000002069</v>
+      </c>
+      <c r="P143">
+        <f t="shared" si="10"/>
+        <v>1133905.5225000007</v>
+      </c>
+      <c r="U143">
+        <f t="shared" si="11"/>
+        <v>515978948.12889993</v>
+      </c>
+      <c r="Z143">
+        <f t="shared" si="12"/>
+        <v>6387613998.5024977</v>
+      </c>
+      <c r="AE143">
+        <f t="shared" si="13"/>
+        <v>63166683447.828934</v>
+      </c>
+    </row>
+    <row r="144" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A144">
+        <f t="shared" si="7"/>
+        <v>2580.6400000000012</v>
+      </c>
+      <c r="F144">
+        <f t="shared" si="8"/>
+        <v>493.72840000000122</v>
+      </c>
+      <c r="K144">
+        <f t="shared" si="9"/>
+        <v>25315.992100000039</v>
+      </c>
+      <c r="P144">
+        <f t="shared" si="10"/>
+        <v>6921371.722500002</v>
+      </c>
+      <c r="U144">
+        <f t="shared" si="11"/>
+        <v>15365067.228900013</v>
+      </c>
+      <c r="Z144">
+        <f t="shared" si="12"/>
+        <v>1108127561.1024992</v>
+      </c>
+      <c r="AE144">
+        <f t="shared" si="13"/>
+        <v>50663180696.128937</v>
+      </c>
+    </row>
+    <row r="145" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A145">
+        <f t="shared" si="7"/>
+        <v>7.8400000000000638</v>
+      </c>
+      <c r="F145">
+        <f t="shared" si="8"/>
+        <v>22867.488400000009</v>
+      </c>
+      <c r="K145">
+        <f t="shared" si="9"/>
+        <v>102970.39209999992</v>
+      </c>
+      <c r="P145">
+        <f t="shared" si="10"/>
+        <v>15156616.922499998</v>
+      </c>
+      <c r="U145">
+        <f t="shared" si="11"/>
+        <v>439328726.42889994</v>
+      </c>
+      <c r="Z145">
+        <f t="shared" si="12"/>
+        <v>4661550727.8024988</v>
+      </c>
+      <c r="AE145">
+        <f t="shared" si="13"/>
+        <v>7360238094.7489128</v>
+      </c>
+    </row>
+    <row r="146" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A146">
+        <f t="shared" si="7"/>
+        <v>475.24000000000052</v>
+      </c>
+      <c r="F146">
+        <f t="shared" si="8"/>
+        <v>8608.1283999999941</v>
+      </c>
+      <c r="K146">
+        <f t="shared" si="9"/>
+        <v>17985.492100000036</v>
+      </c>
+      <c r="P146">
+        <f t="shared" si="10"/>
+        <v>7081.2224999999389</v>
+      </c>
+      <c r="U146">
+        <f t="shared" si="11"/>
+        <v>793.54889999990166</v>
+      </c>
+      <c r="Z146">
+        <f t="shared" si="12"/>
+        <v>2344443138.3025012</v>
+      </c>
+      <c r="AE146">
+        <f t="shared" si="13"/>
+        <v>29048488044.268875</v>
+      </c>
+    </row>
+    <row r="147" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A147">
+        <f t="shared" si="7"/>
+        <v>1036.8399999999992</v>
+      </c>
+      <c r="F147">
+        <f t="shared" si="8"/>
+        <v>29165.808399999991</v>
+      </c>
+      <c r="K147">
+        <f t="shared" si="9"/>
+        <v>79.03209999999774</v>
+      </c>
+      <c r="P147">
+        <f t="shared" si="10"/>
+        <v>649877.82249999943</v>
+      </c>
+      <c r="U147">
+        <f t="shared" si="11"/>
+        <v>11136703.608899988</v>
+      </c>
+      <c r="Z147">
+        <f t="shared" si="12"/>
+        <v>110871423.20249976</v>
+      </c>
+      <c r="AE147">
+        <f t="shared" si="13"/>
+        <v>39472880133.508926</v>
+      </c>
+    </row>
+    <row r="148" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A148">
+        <f t="shared" si="7"/>
+        <v>1211.0400000000009</v>
+      </c>
+      <c r="F148">
+        <f t="shared" si="8"/>
+        <v>39513.488399999987</v>
+      </c>
+      <c r="K148">
+        <f t="shared" si="9"/>
+        <v>59482.332099999941</v>
+      </c>
+      <c r="P148">
+        <f t="shared" si="10"/>
+        <v>1649041.222499999</v>
+      </c>
+      <c r="U148">
+        <f t="shared" si="11"/>
+        <v>250170.02889999826</v>
+      </c>
+      <c r="Z148">
+        <f t="shared" si="12"/>
+        <v>10455198.902500074</v>
+      </c>
+      <c r="AE148">
+        <f t="shared" si="13"/>
+        <v>8159900936.9088869</v>
+      </c>
+    </row>
+    <row r="149" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A149">
+        <f t="shared" si="7"/>
+        <v>635.0399999999994</v>
+      </c>
+      <c r="F149">
+        <f t="shared" si="8"/>
+        <v>6852.5283999999956</v>
+      </c>
+      <c r="K149">
+        <f t="shared" si="9"/>
+        <v>89466.792100000079</v>
+      </c>
+      <c r="P149">
+        <f t="shared" si="10"/>
+        <v>7307019.9224999985</v>
+      </c>
+      <c r="U149">
+        <f t="shared" si="11"/>
+        <v>411772163.30889994</v>
+      </c>
+      <c r="Z149">
+        <f t="shared" si="12"/>
+        <v>259224490.20250037</v>
+      </c>
+      <c r="AE149">
+        <f t="shared" si="13"/>
+        <v>77216644162.168945</v>
+      </c>
+    </row>
+    <row r="150" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A150">
+        <f t="shared" si="7"/>
+        <v>795.23999999999933</v>
+      </c>
+      <c r="F150">
+        <f t="shared" si="8"/>
+        <v>3507.0084000000033</v>
+      </c>
+      <c r="K150">
+        <f t="shared" si="9"/>
+        <v>468006.49210000015</v>
+      </c>
+      <c r="P150">
+        <f t="shared" si="10"/>
+        <v>237315.12249999965</v>
+      </c>
+      <c r="U150">
+        <f t="shared" si="11"/>
+        <v>607105.88889999723</v>
+      </c>
+      <c r="Z150">
+        <f t="shared" si="12"/>
+        <v>2664257910.6025014</v>
+      </c>
+      <c r="AE150">
+        <f t="shared" si="13"/>
+        <v>22251441278.488876</v>
+      </c>
+    </row>
+    <row r="151" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A151">
+        <f t="shared" si="7"/>
+        <v>2097.6400000000012</v>
+      </c>
+      <c r="F151">
+        <f t="shared" si="8"/>
+        <v>10044.048400000005</v>
+      </c>
+      <c r="K151">
+        <f t="shared" si="9"/>
+        <v>142211.95210000008</v>
+      </c>
+      <c r="P151">
+        <f t="shared" si="10"/>
+        <v>19581952.522499997</v>
+      </c>
+      <c r="U151">
+        <f t="shared" si="11"/>
+        <v>5303026.0089000082</v>
+      </c>
+      <c r="Z151">
+        <f t="shared" si="12"/>
+        <v>114416181.90249975</v>
+      </c>
+      <c r="AE151">
+        <f t="shared" si="13"/>
+        <v>20185825622.848923</v>
+      </c>
+    </row>
+    <row r="152" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A152">
+        <f t="shared" si="7"/>
+        <v>718.24000000000058</v>
+      </c>
+      <c r="F152">
+        <f t="shared" si="8"/>
+        <v>31053.488400000009</v>
+      </c>
+      <c r="K152">
+        <f t="shared" si="9"/>
+        <v>636628.45209999976</v>
+      </c>
+      <c r="P152">
+        <f t="shared" si="10"/>
+        <v>8685693.1224999987</v>
+      </c>
+      <c r="U152">
+        <f t="shared" si="11"/>
+        <v>37750824.988899976</v>
+      </c>
+      <c r="Z152">
+        <f t="shared" si="12"/>
+        <v>6483720014.4024982</v>
+      </c>
+      <c r="AE152">
+        <f t="shared" si="13"/>
+        <v>94157640530.368851</v>
+      </c>
+    </row>
+    <row r="153" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A153">
+        <f t="shared" si="7"/>
+        <v>829.44000000000062</v>
+      </c>
+      <c r="F153">
+        <f t="shared" si="8"/>
+        <v>1171.0084000000018</v>
+      </c>
+      <c r="K153">
+        <f t="shared" si="9"/>
+        <v>3613.2121000000152</v>
+      </c>
+      <c r="P153">
+        <f t="shared" si="10"/>
+        <v>5929955.5224999981</v>
+      </c>
+      <c r="U153">
+        <f t="shared" si="11"/>
+        <v>4227835.0688999929</v>
+      </c>
+      <c r="Z153">
+        <f t="shared" si="12"/>
+        <v>36801815.602500141</v>
+      </c>
+      <c r="AE153">
+        <f t="shared" si="13"/>
+        <v>45489284039.908867</v>
+      </c>
+    </row>
+    <row r="154" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A154">
+        <f t="shared" si="7"/>
+        <v>739.83999999999935</v>
+      </c>
+      <c r="F154">
+        <f t="shared" si="8"/>
+        <v>17630.528399999992</v>
+      </c>
+      <c r="K154">
+        <f t="shared" si="9"/>
+        <v>49235.172099999945</v>
+      </c>
+      <c r="P154">
+        <f t="shared" si="10"/>
+        <v>743302.62249999936</v>
+      </c>
+      <c r="U154">
+        <f t="shared" si="11"/>
+        <v>25222191.508899983</v>
+      </c>
+      <c r="Z154">
+        <f t="shared" si="12"/>
+        <v>122046151.50250025</v>
+      </c>
+      <c r="AE154">
+        <f t="shared" si="13"/>
+        <v>68012900179.408936</v>
+      </c>
+    </row>
+    <row r="155" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A155">
+        <f t="shared" si="7"/>
+        <v>249.64000000000036</v>
+      </c>
+      <c r="F155">
+        <f t="shared" si="8"/>
+        <v>331.968400000001</v>
+      </c>
+      <c r="K155">
+        <f t="shared" si="9"/>
+        <v>630.5121000000064</v>
+      </c>
+      <c r="P155">
+        <f t="shared" si="10"/>
+        <v>7844760.722500002</v>
+      </c>
+      <c r="U155">
+        <f t="shared" si="11"/>
+        <v>256197478.06889993</v>
+      </c>
+      <c r="Z155">
+        <f t="shared" si="12"/>
+        <v>327011163.90250045</v>
+      </c>
+      <c r="AE155">
+        <f t="shared" si="13"/>
+        <v>2659791863.8488922</v>
+      </c>
+    </row>
+    <row r="156" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A156">
+        <f t="shared" si="7"/>
+        <v>1142.4400000000007</v>
+      </c>
+      <c r="F156">
+        <f t="shared" si="8"/>
+        <v>3747.8884000000035</v>
+      </c>
+      <c r="K156">
+        <f t="shared" si="9"/>
+        <v>1793215.5921000002</v>
+      </c>
+      <c r="P156">
+        <f t="shared" si="10"/>
+        <v>619605.12249999947</v>
+      </c>
+      <c r="U156">
+        <f t="shared" si="11"/>
+        <v>76758099.768899962</v>
+      </c>
+      <c r="Z156">
+        <f t="shared" si="12"/>
+        <v>220506165.30250034</v>
+      </c>
+      <c r="AE156">
+        <f t="shared" si="13"/>
+        <v>3395412711.8288913</v>
+      </c>
+    </row>
+    <row r="157" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A157">
+        <f t="shared" si="7"/>
+        <v>2830.2399999999989</v>
+      </c>
+      <c r="F157">
+        <f t="shared" si="8"/>
+        <v>3816.7683999999967</v>
+      </c>
+      <c r="K157">
+        <f t="shared" si="9"/>
+        <v>179022.07210000011</v>
+      </c>
+      <c r="P157">
+        <f t="shared" si="10"/>
+        <v>2386561.5225000009</v>
+      </c>
+      <c r="U157">
+        <f t="shared" si="11"/>
+        <v>56879199.748900026</v>
+      </c>
+      <c r="Z157">
+        <f t="shared" si="12"/>
+        <v>236312219.00250036</v>
+      </c>
+      <c r="AE157">
+        <f t="shared" si="13"/>
+        <v>36821069785.948868</v>
+      </c>
+    </row>
+    <row r="158" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A158">
+        <f t="shared" si="7"/>
+        <v>282.24000000000041</v>
+      </c>
+      <c r="F158">
+        <f t="shared" si="8"/>
+        <v>19259.888399999993</v>
+      </c>
+      <c r="K158">
+        <f t="shared" si="9"/>
+        <v>771077.1721000002</v>
+      </c>
+      <c r="P158">
+        <f t="shared" si="10"/>
+        <v>3821438.5225000014</v>
+      </c>
+      <c r="U158">
+        <f t="shared" si="11"/>
+        <v>7751602.5888999905</v>
+      </c>
+      <c r="Z158">
+        <f t="shared" si="12"/>
+        <v>9464069643.9025021</v>
+      </c>
+      <c r="AE158">
+        <f t="shared" si="13"/>
+        <v>133057276921.82884</v>
+      </c>
+    </row>
+    <row r="159" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A159">
+        <f t="shared" si="7"/>
+        <v>1780.839999999999</v>
+      </c>
+      <c r="F159">
+        <f t="shared" si="8"/>
+        <v>352.68839999999898</v>
+      </c>
+      <c r="K159">
+        <f t="shared" si="9"/>
+        <v>99786.492099999916</v>
+      </c>
+      <c r="P159">
+        <f t="shared" si="10"/>
+        <v>15838.222500000091</v>
+      </c>
+      <c r="U159">
+        <f t="shared" si="11"/>
+        <v>2283634.7688999949</v>
+      </c>
+      <c r="Z159">
+        <f t="shared" si="12"/>
+        <v>46791756.202500157</v>
+      </c>
+      <c r="AE159">
+        <f t="shared" si="13"/>
+        <v>17553115189.948879</v>
+      </c>
+    </row>
+    <row r="160" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A160">
+        <f t="shared" si="7"/>
+        <v>1953.639999999999</v>
+      </c>
+      <c r="F160">
+        <f t="shared" si="8"/>
+        <v>11616.528399999994</v>
+      </c>
+      <c r="K160">
+        <f t="shared" si="9"/>
+        <v>151406.5921000001</v>
+      </c>
+      <c r="P160">
+        <f t="shared" si="10"/>
+        <v>3693507.4225000013</v>
+      </c>
+      <c r="U160">
+        <f t="shared" si="11"/>
+        <v>85263616.468900025</v>
+      </c>
+      <c r="Z160">
+        <f t="shared" si="12"/>
+        <v>2468147112.2025013</v>
+      </c>
+      <c r="AE160">
+        <f t="shared" si="13"/>
+        <v>986850076.78889537</v>
+      </c>
+    </row>
+    <row r="161" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A161">
+        <f t="shared" si="7"/>
+        <v>17.639999999999905</v>
+      </c>
+      <c r="F161">
+        <f t="shared" si="8"/>
+        <v>2325.1684000000027</v>
+      </c>
+      <c r="K161">
+        <f t="shared" si="9"/>
+        <v>19630.812100000036</v>
+      </c>
+      <c r="P161">
+        <f t="shared" si="10"/>
+        <v>41677.222499999851</v>
+      </c>
+      <c r="U161">
+        <f t="shared" si="11"/>
+        <v>632983835.08889997</v>
+      </c>
+      <c r="Z161">
+        <f t="shared" si="12"/>
+        <v>53356450.702499829</v>
+      </c>
+      <c r="AE161">
+        <f t="shared" si="13"/>
+        <v>2114880508.1089067</v>
+      </c>
+    </row>
+    <row r="162" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A162">
+        <f t="shared" si="7"/>
+        <v>3271.8399999999988</v>
+      </c>
+      <c r="F162">
+        <f t="shared" si="8"/>
+        <v>7530.7683999999954</v>
+      </c>
+      <c r="K162">
+        <f t="shared" si="9"/>
+        <v>1713193.0320999997</v>
+      </c>
+      <c r="P162">
+        <f t="shared" si="10"/>
+        <v>2832993.9224999989</v>
+      </c>
+      <c r="U162">
+        <f t="shared" si="11"/>
+        <v>470550239.30889994</v>
+      </c>
+      <c r="Z162">
+        <f t="shared" si="12"/>
+        <v>3406525753.7025013</v>
+      </c>
+      <c r="AE162">
+        <f t="shared" si="13"/>
+        <v>859417888.58890438</v>
+      </c>
+    </row>
+    <row r="163" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A163">
+        <f t="shared" si="7"/>
+        <v>566.44000000000051</v>
+      </c>
+      <c r="F163">
+        <f t="shared" si="8"/>
+        <v>5508.6084000000037</v>
+      </c>
+      <c r="K163">
+        <f t="shared" si="9"/>
+        <v>28598.192100000044</v>
+      </c>
+      <c r="P163">
+        <f t="shared" si="10"/>
+        <v>350286.42250000045</v>
+      </c>
+      <c r="U163">
+        <f t="shared" si="11"/>
+        <v>39553659.28889998</v>
+      </c>
+      <c r="Z163">
+        <f t="shared" si="12"/>
+        <v>5632720147.1025019</v>
+      </c>
+      <c r="AE163">
+        <f t="shared" si="13"/>
+        <v>12178850642.308916</v>
+      </c>
+    </row>
+    <row r="164" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A164">
+        <f t="shared" si="7"/>
+        <v>4.8399999999999501</v>
+      </c>
+      <c r="F164">
+        <f t="shared" si="8"/>
+        <v>281.56839999999909</v>
+      </c>
+      <c r="K164">
+        <f t="shared" si="9"/>
+        <v>201502.23209999988</v>
+      </c>
+      <c r="P164">
+        <f t="shared" si="10"/>
+        <v>8381893.5224999981</v>
+      </c>
+      <c r="U164">
+        <f t="shared" si="11"/>
+        <v>145182497.68889996</v>
+      </c>
+      <c r="Z164">
+        <f t="shared" si="12"/>
+        <v>1315407719.1024992</v>
+      </c>
+      <c r="AE164">
+        <f t="shared" si="13"/>
+        <v>3372028504.4888911</v>
+      </c>
+    </row>
+    <row r="165" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A165">
+        <f t="shared" si="7"/>
+        <v>10.239999999999927</v>
+      </c>
+      <c r="F165">
+        <f t="shared" si="8"/>
+        <v>9956.0483999999942</v>
+      </c>
+      <c r="K165">
+        <f t="shared" si="9"/>
+        <v>678794.73209999979</v>
+      </c>
+      <c r="P165">
+        <f t="shared" si="10"/>
+        <v>675930.62249999936</v>
+      </c>
+      <c r="U165">
+        <f t="shared" si="11"/>
+        <v>103445782.88890004</v>
+      </c>
+      <c r="Z165">
+        <f t="shared" si="12"/>
+        <v>1744603415.4025009</v>
+      </c>
+      <c r="AE165">
+        <f t="shared" si="13"/>
+        <v>879844329.10889554</v>
+      </c>
+    </row>
+    <row r="166" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A166">
+        <f t="shared" si="7"/>
+        <v>67.23999999999981</v>
+      </c>
+      <c r="F166">
+        <f t="shared" si="8"/>
+        <v>65137.248400000011</v>
+      </c>
+      <c r="K166">
+        <f t="shared" si="9"/>
+        <v>53875.052100000059</v>
+      </c>
+      <c r="P166">
+        <f t="shared" si="10"/>
+        <v>26634372.722500004</v>
+      </c>
+      <c r="U166">
+        <f t="shared" si="11"/>
+        <v>318509341.04890007</v>
+      </c>
+      <c r="Z166">
+        <f t="shared" si="12"/>
+        <v>1433489396.1025009</v>
+      </c>
+      <c r="AE166">
+        <f t="shared" si="13"/>
+        <v>2230311132.8688931</v>
+      </c>
+    </row>
+    <row r="167" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A167">
+        <f t="shared" si="7"/>
+        <v>519.84000000000049</v>
+      </c>
+      <c r="F167">
+        <f t="shared" si="8"/>
+        <v>4518.5284000000038</v>
+      </c>
+      <c r="K167">
+        <f t="shared" si="9"/>
+        <v>101054.05209999991</v>
+      </c>
+      <c r="P167">
+        <f t="shared" si="10"/>
+        <v>281801.72250000038</v>
+      </c>
+      <c r="U167">
+        <f t="shared" si="11"/>
+        <v>176761545.32889995</v>
+      </c>
+      <c r="Z167">
+        <f t="shared" si="12"/>
+        <v>699631595.30249941</v>
+      </c>
+      <c r="AE167">
+        <f t="shared" si="13"/>
+        <v>3978477070.5288906</v>
+      </c>
+    </row>
+    <row r="168" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A168">
+        <f t="shared" si="7"/>
+        <v>46.240000000000151</v>
+      </c>
+      <c r="F168">
+        <f t="shared" si="8"/>
+        <v>1503.8883999999978</v>
+      </c>
+      <c r="K168">
+        <f t="shared" si="9"/>
+        <v>761936.95209999976</v>
+      </c>
+      <c r="P168">
+        <f t="shared" si="10"/>
+        <v>8306788.6224999977</v>
+      </c>
+      <c r="U168">
+        <f t="shared" si="11"/>
+        <v>126311299.76890004</v>
+      </c>
+      <c r="Z168">
+        <f t="shared" si="12"/>
+        <v>484992708.50249946</v>
+      </c>
+      <c r="AE168">
+        <f t="shared" si="13"/>
+        <v>13272383265.988916</v>
+      </c>
+    </row>
+    <row r="169" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A169">
+        <f t="shared" si="7"/>
+        <v>585.63999999999942</v>
+      </c>
+      <c r="F169">
+        <f t="shared" si="8"/>
+        <v>25991.888400000007</v>
+      </c>
+      <c r="K169">
+        <f t="shared" si="9"/>
+        <v>189129.31209999989</v>
+      </c>
+      <c r="P169">
+        <f t="shared" si="10"/>
+        <v>13748151.622500002</v>
+      </c>
+      <c r="U169">
+        <f t="shared" si="11"/>
+        <v>25645817.78889998</v>
+      </c>
+      <c r="Z169">
+        <f t="shared" si="12"/>
+        <v>4822406636.6024981</v>
+      </c>
+      <c r="AE169">
+        <f t="shared" si="13"/>
+        <v>159007009471.64896</v>
+      </c>
+    </row>
+    <row r="170" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A170">
+        <f t="shared" ref="A170:A204" si="14">($A66-$A$102)^2</f>
+        <v>1211.0400000000009</v>
+      </c>
+      <c r="F170">
+        <f t="shared" ref="F170:F204" si="15">($F66-$F$102)^2</f>
+        <v>27297.648400000009</v>
+      </c>
+      <c r="K170">
+        <f t="shared" ref="K170:K204" si="16">($K66-$K$102)^2</f>
+        <v>47912.832099999941</v>
+      </c>
+      <c r="P170">
+        <f t="shared" ref="P170:P204" si="17">($P66-$P$102)^2</f>
+        <v>44037.022500000152</v>
+      </c>
+      <c r="U170">
+        <f t="shared" ref="U170:U204" si="18">($U66-$U$102)^2</f>
+        <v>1016769927.4489001</v>
+      </c>
+      <c r="Z170">
+        <f t="shared" ref="Z170:Z204" si="19">($Z66-$Z$102)^2</f>
+        <v>9797347240.4024982</v>
+      </c>
+      <c r="AE170">
+        <f t="shared" ref="AE170:AE204" si="20">($AE66-$AE$102)^2</f>
+        <v>9062691571.3488865</v>
+      </c>
+    </row>
+    <row r="171" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A171">
+        <f t="shared" si="14"/>
+        <v>973.43999999999926</v>
+      </c>
+      <c r="F171">
+        <f t="shared" si="15"/>
+        <v>26315.328400000009</v>
+      </c>
+      <c r="K171">
+        <f t="shared" si="16"/>
+        <v>3613.2121000000152</v>
+      </c>
+      <c r="P171">
+        <f t="shared" si="17"/>
+        <v>4923295.3225000016</v>
+      </c>
+      <c r="U171">
+        <f t="shared" si="18"/>
+        <v>40375476.388899975</v>
+      </c>
+      <c r="Z171">
+        <f t="shared" si="19"/>
+        <v>9563865.5024999287</v>
+      </c>
+      <c r="AE171">
+        <f t="shared" si="20"/>
+        <v>39037789222.828926</v>
+      </c>
+    </row>
+    <row r="172" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A172">
+        <f t="shared" si="14"/>
+        <v>449.43999999999954</v>
+      </c>
+      <c r="F172">
+        <f t="shared" si="15"/>
+        <v>12369.888400000005</v>
+      </c>
+      <c r="K172">
+        <f t="shared" si="16"/>
+        <v>5168.1720999999816</v>
+      </c>
+      <c r="P172">
+        <f t="shared" si="17"/>
+        <v>5088859.222500002</v>
+      </c>
+      <c r="U172">
+        <f t="shared" si="18"/>
+        <v>13580477.928899987</v>
+      </c>
+      <c r="Z172">
+        <f t="shared" si="19"/>
+        <v>1276386374.9024992</v>
+      </c>
+      <c r="AE172">
+        <f t="shared" si="20"/>
+        <v>67987000701.648865</v>
+      </c>
+    </row>
+    <row r="173" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A173">
+        <f t="shared" si="14"/>
+        <v>948.64000000000067</v>
+      </c>
+      <c r="F173">
+        <f t="shared" si="15"/>
+        <v>174.76840000000072</v>
+      </c>
+      <c r="K173">
+        <f t="shared" si="16"/>
+        <v>31290.072099999954</v>
+      </c>
+      <c r="P173">
+        <f t="shared" si="17"/>
+        <v>2028203.222499999</v>
+      </c>
+      <c r="U173">
+        <f t="shared" si="18"/>
+        <v>311175597.62889993</v>
+      </c>
+      <c r="Z173">
+        <f t="shared" si="19"/>
+        <v>4613472798.5024986</v>
+      </c>
+      <c r="AE173">
+        <f t="shared" si="20"/>
+        <v>18389212342.648922</v>
+      </c>
+    </row>
+    <row r="174" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A174">
+        <f t="shared" si="14"/>
+        <v>392.04000000000048</v>
+      </c>
+      <c r="F174">
+        <f t="shared" si="15"/>
+        <v>2478.0483999999974</v>
+      </c>
+      <c r="K174">
+        <f t="shared" si="16"/>
+        <v>446370.97210000019</v>
+      </c>
+      <c r="P174">
+        <f t="shared" si="17"/>
+        <v>2502249.4225000013</v>
+      </c>
+      <c r="U174">
+        <f t="shared" si="18"/>
+        <v>163716375.32889995</v>
+      </c>
+      <c r="Z174">
+        <f t="shared" si="19"/>
+        <v>214840840.50250036</v>
+      </c>
+      <c r="AE174">
+        <f t="shared" si="20"/>
+        <v>20488249435.608879</v>
+      </c>
+    </row>
+    <row r="175" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A175">
+        <f t="shared" si="14"/>
+        <v>1953.639999999999</v>
+      </c>
+      <c r="F175">
+        <f t="shared" si="15"/>
+        <v>21251.808399999991</v>
+      </c>
+      <c r="K175">
+        <f t="shared" si="16"/>
+        <v>415883.11209999985</v>
+      </c>
+      <c r="P175">
+        <f t="shared" si="17"/>
+        <v>1954823.4224999989</v>
+      </c>
+      <c r="U175">
+        <f t="shared" si="18"/>
+        <v>8507897.2489000093</v>
+      </c>
+      <c r="Z175">
+        <f t="shared" si="19"/>
+        <v>498425717.70250052</v>
+      </c>
+      <c r="AE175">
+        <f t="shared" si="20"/>
+        <v>3598659724.768909</v>
+      </c>
+    </row>
+    <row r="176" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A176">
+        <f t="shared" si="14"/>
+        <v>888.04000000000065</v>
+      </c>
+      <c r="F176">
+        <f t="shared" si="15"/>
+        <v>23037.168399999991</v>
+      </c>
+      <c r="K176">
+        <f t="shared" si="16"/>
+        <v>334211.17210000014</v>
+      </c>
+      <c r="P176">
+        <f t="shared" si="17"/>
+        <v>4818683.5224999981</v>
+      </c>
+      <c r="U176">
+        <f t="shared" si="18"/>
+        <v>27585289.708899982</v>
+      </c>
+      <c r="Z176">
+        <f t="shared" si="19"/>
+        <v>4531504440.6025019</v>
+      </c>
+      <c r="AE176">
+        <f t="shared" si="20"/>
+        <v>80281459264.42894</v>
+      </c>
+    </row>
+    <row r="177" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A177">
+        <f t="shared" si="14"/>
+        <v>316.84000000000043</v>
+      </c>
+      <c r="F177">
+        <f t="shared" si="15"/>
+        <v>9560.9283999999952</v>
+      </c>
+      <c r="K177">
+        <f t="shared" si="16"/>
+        <v>128085.25209999991</v>
+      </c>
+      <c r="P177">
+        <f t="shared" si="17"/>
+        <v>4116232.3225000016</v>
+      </c>
+      <c r="U177">
+        <f t="shared" si="18"/>
+        <v>462930940.58890009</v>
+      </c>
+      <c r="Z177">
+        <f t="shared" si="19"/>
+        <v>3083075597.7025013</v>
+      </c>
+      <c r="AE177">
+        <f t="shared" si="20"/>
+        <v>32624606717.208927</v>
+      </c>
+    </row>
+    <row r="178" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A178">
+        <f t="shared" si="14"/>
+        <v>795.23999999999933</v>
+      </c>
+      <c r="F178">
+        <f t="shared" si="15"/>
+        <v>1427.3283999999978</v>
+      </c>
+      <c r="K178">
+        <f t="shared" si="16"/>
+        <v>4110.0921000000162</v>
+      </c>
+      <c r="P178">
+        <f t="shared" si="17"/>
+        <v>5428201.0225000018</v>
+      </c>
+      <c r="U178">
+        <f t="shared" si="18"/>
+        <v>179886304.10889995</v>
+      </c>
+      <c r="Z178">
+        <f t="shared" si="19"/>
+        <v>467015871.30249947</v>
+      </c>
+      <c r="AE178">
+        <f t="shared" si="20"/>
+        <v>137140731535.52884</v>
+      </c>
+    </row>
+    <row r="179" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A179">
+        <f t="shared" si="14"/>
+        <v>1011.2400000000007</v>
+      </c>
+      <c r="F179">
+        <f t="shared" si="15"/>
+        <v>60900.368399999985</v>
+      </c>
+      <c r="K179">
+        <f t="shared" si="16"/>
+        <v>530144.1721000002</v>
+      </c>
+      <c r="P179">
+        <f t="shared" si="17"/>
+        <v>45731.822500000155</v>
+      </c>
+      <c r="U179">
+        <f t="shared" si="18"/>
+        <v>1584652.9689000044</v>
+      </c>
+      <c r="Z179">
+        <f t="shared" si="19"/>
+        <v>258420092.70250037</v>
+      </c>
+      <c r="AE179">
+        <f t="shared" si="20"/>
+        <v>226718368.40889776</v>
+      </c>
+    </row>
+    <row r="180" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A180">
+        <f t="shared" si="14"/>
+        <v>1459.2399999999991</v>
+      </c>
+      <c r="F180">
+        <f t="shared" si="15"/>
+        <v>4869.2483999999959</v>
+      </c>
+      <c r="K180">
+        <f t="shared" si="16"/>
+        <v>3351.2520999999851</v>
+      </c>
+      <c r="P180">
+        <f t="shared" si="17"/>
+        <v>84593.722500000207</v>
+      </c>
+      <c r="U180">
+        <f t="shared" si="18"/>
+        <v>289810787.86890006</v>
+      </c>
+      <c r="Z180">
+        <f t="shared" si="19"/>
+        <v>58345918.402500175</v>
+      </c>
+      <c r="AE180">
+        <f t="shared" si="20"/>
+        <v>5313851600.668889</v>
+      </c>
+    </row>
+    <row r="181" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A181">
+        <f t="shared" si="14"/>
+        <v>686.43999999999937</v>
+      </c>
+      <c r="F181">
+        <f t="shared" si="15"/>
+        <v>1745.5683999999976</v>
+      </c>
+      <c r="K181">
+        <f t="shared" si="16"/>
+        <v>149080.93210000009</v>
+      </c>
+      <c r="P181">
+        <f t="shared" si="17"/>
+        <v>7766532.9225000022</v>
+      </c>
+      <c r="U181">
+        <f t="shared" si="18"/>
+        <v>388201510.00890005</v>
+      </c>
+      <c r="Z181">
+        <f t="shared" si="19"/>
+        <v>1639484639.3024991</v>
+      </c>
+      <c r="AE181">
+        <f t="shared" si="20"/>
+        <v>4484333993.12889</v>
+      </c>
+    </row>
+    <row r="182" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A182">
+        <f t="shared" si="14"/>
+        <v>84.639999999999787</v>
+      </c>
+      <c r="F182">
+        <f t="shared" si="15"/>
+        <v>586.60840000000132</v>
+      </c>
+      <c r="K182">
+        <f t="shared" si="16"/>
+        <v>7763.3721000000223</v>
+      </c>
+      <c r="P182">
+        <f t="shared" si="17"/>
+        <v>2100035.7224999988</v>
+      </c>
+      <c r="U182">
+        <f t="shared" si="18"/>
+        <v>109101576.32889996</v>
+      </c>
+      <c r="Z182">
+        <f t="shared" si="19"/>
+        <v>3648347242.4024987</v>
+      </c>
+      <c r="AE182">
+        <f t="shared" si="20"/>
+        <v>28316196289.188873</v>
+      </c>
+    </row>
+    <row r="183" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A183">
+        <f t="shared" si="14"/>
+        <v>4.8399999999999501</v>
+      </c>
+      <c r="F183">
+        <f t="shared" si="15"/>
+        <v>3223.968399999997</v>
+      </c>
+      <c r="K183">
+        <f t="shared" si="16"/>
+        <v>51026.292099999941</v>
+      </c>
+      <c r="P183">
+        <f t="shared" si="17"/>
+        <v>1136675.8224999993</v>
+      </c>
+      <c r="U183">
+        <f t="shared" si="18"/>
+        <v>71382728.368900031</v>
+      </c>
+      <c r="Z183">
+        <f t="shared" si="19"/>
+        <v>815185297.10250068</v>
+      </c>
+      <c r="AE183">
+        <f t="shared" si="20"/>
+        <v>43832518227.108871</v>
+      </c>
+    </row>
+    <row r="184" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A184">
+        <f t="shared" si="14"/>
+        <v>772.8400000000006</v>
+      </c>
+      <c r="F184">
+        <f t="shared" si="15"/>
+        <v>60.528399999999579</v>
+      </c>
+      <c r="K184">
+        <f t="shared" si="16"/>
+        <v>22834.232100000037</v>
+      </c>
+      <c r="P184">
+        <f t="shared" si="17"/>
+        <v>1928904.3225000009</v>
+      </c>
+      <c r="U184">
+        <f t="shared" si="18"/>
+        <v>110737106.84889996</v>
+      </c>
+      <c r="Z184">
+        <f t="shared" si="19"/>
+        <v>43843600.102500156</v>
+      </c>
+      <c r="AE184">
+        <f t="shared" si="20"/>
+        <v>19487369872.008881</v>
+      </c>
+    </row>
+    <row r="185" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A185">
+        <f t="shared" si="14"/>
+        <v>1505.440000000001</v>
+      </c>
+      <c r="F185">
+        <f t="shared" si="15"/>
+        <v>42757.968399999991</v>
+      </c>
+      <c r="K185">
+        <f t="shared" si="16"/>
+        <v>3123.6920999999857</v>
+      </c>
+      <c r="P185">
+        <f t="shared" si="17"/>
+        <v>7242288.3224999979</v>
+      </c>
+      <c r="U185">
+        <f t="shared" si="18"/>
+        <v>588442316.30890012</v>
+      </c>
+      <c r="Z185">
+        <f t="shared" si="19"/>
+        <v>35300828.102500141</v>
+      </c>
+      <c r="AE185">
+        <f t="shared" si="20"/>
+        <v>13290130892.808918</v>
+      </c>
+    </row>
+    <row r="186" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A186">
+        <f t="shared" si="14"/>
+        <v>2381.440000000001</v>
+      </c>
+      <c r="F186">
+        <f t="shared" si="15"/>
+        <v>8060.4483999999948</v>
+      </c>
+      <c r="K186">
+        <f t="shared" si="16"/>
+        <v>630.5121000000064</v>
+      </c>
+      <c r="P186">
+        <f t="shared" si="17"/>
+        <v>1466884.3224999991</v>
+      </c>
+      <c r="U186">
+        <f t="shared" si="18"/>
+        <v>5312241.3289000085</v>
+      </c>
+      <c r="Z186">
+        <f t="shared" si="19"/>
+        <v>310903293.00250041</v>
+      </c>
+      <c r="AE186">
+        <f t="shared" si="20"/>
+        <v>2661407380.7689075</v>
+      </c>
+    </row>
+    <row r="187" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A187">
+        <f t="shared" si="14"/>
+        <v>148.83999999999972</v>
+      </c>
+      <c r="F187">
+        <f t="shared" si="15"/>
+        <v>131203.32840000003</v>
+      </c>
+      <c r="K187">
+        <f t="shared" si="16"/>
+        <v>917974.77210000029</v>
+      </c>
+      <c r="P187">
+        <f t="shared" si="17"/>
+        <v>8380156.5225000018</v>
+      </c>
+      <c r="U187">
+        <f t="shared" si="18"/>
+        <v>8989023.3488999903</v>
+      </c>
+      <c r="Z187">
+        <f t="shared" si="19"/>
+        <v>789078999.30249929</v>
+      </c>
+      <c r="AE187">
+        <f t="shared" si="20"/>
+        <v>91027011268.648941</v>
+      </c>
+    </row>
+    <row r="188" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A188">
+        <f t="shared" si="14"/>
+        <v>10.239999999999927</v>
+      </c>
+      <c r="F188">
+        <f t="shared" si="15"/>
+        <v>6525.4083999999957</v>
+      </c>
+      <c r="K188">
+        <f t="shared" si="16"/>
+        <v>20417.552099999964</v>
+      </c>
+      <c r="P188">
+        <f t="shared" si="17"/>
+        <v>1771960.3224999991</v>
+      </c>
+      <c r="U188">
+        <f t="shared" si="18"/>
+        <v>317653269.20890003</v>
+      </c>
+      <c r="Z188">
+        <f t="shared" si="19"/>
+        <v>654154794.60250056</v>
+      </c>
+      <c r="AE188">
+        <f t="shared" si="20"/>
+        <v>3352506114.6889086</v>
+      </c>
+    </row>
+    <row r="189" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A189">
+        <f t="shared" si="14"/>
+        <v>125.43999999999974</v>
+      </c>
+      <c r="F189">
+        <f t="shared" si="15"/>
+        <v>1617.6484000000021</v>
+      </c>
+      <c r="K189">
+        <f t="shared" si="16"/>
+        <v>180718.51210000011</v>
+      </c>
+      <c r="P189">
+        <f t="shared" si="17"/>
+        <v>387942.12250000046</v>
+      </c>
+      <c r="U189">
+        <f t="shared" si="18"/>
+        <v>229406465.66889995</v>
+      </c>
+      <c r="Z189">
+        <f t="shared" si="19"/>
+        <v>6456532291.5024977</v>
+      </c>
+      <c r="AE189">
+        <f t="shared" si="20"/>
+        <v>2386925347.068893</v>
+      </c>
+    </row>
+    <row r="190" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A190">
+        <f t="shared" si="14"/>
+        <v>96.040000000000219</v>
+      </c>
+      <c r="F190">
+        <f t="shared" si="15"/>
+        <v>1663.0083999999977</v>
+      </c>
+      <c r="K190">
+        <f t="shared" si="16"/>
+        <v>371014.99210000015</v>
+      </c>
+      <c r="P190">
+        <f t="shared" si="17"/>
+        <v>1600604.522499999</v>
+      </c>
+      <c r="U190">
+        <f t="shared" si="18"/>
+        <v>12157983.448900012</v>
+      </c>
+      <c r="Z190">
+        <f t="shared" si="19"/>
+        <v>1659132483.002501</v>
+      </c>
+      <c r="AE190">
+        <f t="shared" si="20"/>
+        <v>83350675184.728851</v>
+      </c>
+    </row>
+    <row r="191" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A191">
+        <f t="shared" si="14"/>
+        <v>1.4399999999999726</v>
+      </c>
+      <c r="F191">
+        <f t="shared" si="15"/>
+        <v>20511.968400000009</v>
+      </c>
+      <c r="K191">
+        <f t="shared" si="16"/>
+        <v>10022.012100000025</v>
+      </c>
+      <c r="P191">
+        <f t="shared" si="17"/>
+        <v>79439.422500000204</v>
+      </c>
+      <c r="U191">
+        <f t="shared" si="18"/>
+        <v>5432768.4889000077</v>
+      </c>
+      <c r="Z191">
+        <f t="shared" si="19"/>
+        <v>8913163131.2024975</v>
+      </c>
+      <c r="AE191">
+        <f t="shared" si="20"/>
+        <v>27884046999.928875</v>
+      </c>
+    </row>
+    <row r="192" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A192">
+        <f t="shared" si="14"/>
+        <v>3819.2400000000016</v>
+      </c>
+      <c r="F192">
+        <f t="shared" si="15"/>
+        <v>8423.5683999999947</v>
+      </c>
+      <c r="K192">
+        <f t="shared" si="16"/>
+        <v>22467.012099999964</v>
+      </c>
+      <c r="P192">
+        <f t="shared" si="17"/>
+        <v>10589492.222499998</v>
+      </c>
+      <c r="U192">
+        <f t="shared" si="18"/>
+        <v>35798323.248899981</v>
+      </c>
+      <c r="Z192">
+        <f t="shared" si="19"/>
+        <v>642442527.60250056</v>
+      </c>
+      <c r="AE192">
+        <f t="shared" si="20"/>
+        <v>12248329212.508884</v>
+      </c>
+    </row>
+    <row r="193" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A193">
+        <f t="shared" si="14"/>
+        <v>116.64000000000024</v>
+      </c>
+      <c r="F193">
+        <f t="shared" si="15"/>
+        <v>19259.888399999993</v>
+      </c>
+      <c r="K193">
+        <f t="shared" si="16"/>
+        <v>156728.89209999991</v>
+      </c>
+      <c r="P193">
+        <f t="shared" si="17"/>
+        <v>779953.9224999994</v>
+      </c>
+      <c r="U193">
+        <f t="shared" si="18"/>
+        <v>42213218.008899979</v>
+      </c>
+      <c r="Z193">
+        <f t="shared" si="19"/>
+        <v>203021177.10249966</v>
+      </c>
+      <c r="AE193">
+        <f t="shared" si="20"/>
+        <v>19431962.748899344</v>
+      </c>
+    </row>
+    <row r="194" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A194">
+        <f t="shared" si="14"/>
+        <v>665.64000000000055</v>
+      </c>
+      <c r="F194">
+        <f t="shared" si="15"/>
+        <v>16697.808400000005</v>
+      </c>
+      <c r="K194">
+        <f t="shared" si="16"/>
+        <v>9582.452099999975</v>
+      </c>
+      <c r="P194">
+        <f t="shared" si="17"/>
+        <v>1679227.2225000008</v>
+      </c>
+      <c r="U194">
+        <f t="shared" si="18"/>
+        <v>92003202.748900026</v>
+      </c>
+      <c r="Z194">
+        <f t="shared" si="19"/>
+        <v>152484217.4025003</v>
+      </c>
+      <c r="AE194">
+        <f t="shared" si="20"/>
+        <v>31209875634.448875</v>
+      </c>
+    </row>
+    <row r="195" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A195">
+        <f t="shared" si="14"/>
+        <v>262.43999999999966</v>
+      </c>
+      <c r="F195">
+        <f t="shared" si="15"/>
+        <v>40489.488400000009</v>
+      </c>
+      <c r="K195">
+        <f t="shared" si="16"/>
+        <v>1070997.3120999997</v>
+      </c>
+      <c r="P195">
+        <f t="shared" si="17"/>
+        <v>2337382.3225000012</v>
+      </c>
+      <c r="U195">
+        <f t="shared" si="18"/>
+        <v>4738588.848900008</v>
+      </c>
+      <c r="Z195">
+        <f t="shared" si="19"/>
+        <v>6243283308.8025017</v>
+      </c>
+      <c r="AE195">
+        <f t="shared" si="20"/>
+        <v>2787610852.7089081</v>
+      </c>
+    </row>
+    <row r="196" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A196">
+        <f t="shared" si="14"/>
+        <v>125.43999999999974</v>
+      </c>
+      <c r="F196">
+        <f t="shared" si="15"/>
+        <v>10978.848399999993</v>
+      </c>
+      <c r="K196">
+        <f t="shared" si="16"/>
+        <v>127527.55210000009</v>
+      </c>
+      <c r="P196">
+        <f t="shared" si="17"/>
+        <v>5079839.8225000016</v>
+      </c>
+      <c r="U196">
+        <f t="shared" si="18"/>
+        <v>202175126.56890005</v>
+      </c>
+      <c r="Z196">
+        <f t="shared" si="19"/>
+        <v>1034551843.8025007</v>
+      </c>
+      <c r="AE196">
+        <f t="shared" si="20"/>
+        <v>195676910915.66898</v>
+      </c>
+    </row>
+    <row r="197" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A197">
+        <f t="shared" si="14"/>
+        <v>353.44000000000045</v>
+      </c>
+      <c r="F197">
+        <f t="shared" si="15"/>
+        <v>4124.2084000000032</v>
+      </c>
+      <c r="K197">
+        <f t="shared" si="16"/>
+        <v>22834.232100000037</v>
+      </c>
+      <c r="P197">
+        <f t="shared" si="17"/>
+        <v>2129118.7224999988</v>
+      </c>
+      <c r="U197">
+        <f t="shared" si="18"/>
+        <v>900169808.00890005</v>
+      </c>
+      <c r="Z197">
+        <f t="shared" si="19"/>
+        <v>8384048503.8025017</v>
+      </c>
+      <c r="AE197">
+        <f t="shared" si="20"/>
+        <v>1680740070.0489061</v>
+      </c>
+    </row>
+    <row r="198" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A198">
+        <f t="shared" si="14"/>
+        <v>1866.2399999999991</v>
+      </c>
+      <c r="F198">
+        <f t="shared" si="15"/>
+        <v>16440.368400000007</v>
+      </c>
+      <c r="K198">
+        <f t="shared" si="16"/>
+        <v>935301.75210000027</v>
+      </c>
+      <c r="P198">
+        <f t="shared" si="17"/>
+        <v>6652014.7224999983</v>
+      </c>
+      <c r="U198">
+        <f t="shared" si="18"/>
+        <v>137526516.20889995</v>
+      </c>
+      <c r="Z198">
+        <f t="shared" si="19"/>
+        <v>1138627166.6024992</v>
+      </c>
+      <c r="AE198">
+        <f t="shared" si="20"/>
+        <v>32018152934.268875</v>
+      </c>
+    </row>
+    <row r="199" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A199">
+        <f t="shared" si="14"/>
+        <v>566.44000000000051</v>
+      </c>
+      <c r="F199">
+        <f t="shared" si="15"/>
+        <v>16184.928400000006</v>
+      </c>
+      <c r="K199">
+        <f t="shared" si="16"/>
+        <v>261233.43210000012</v>
+      </c>
+      <c r="P199">
+        <f t="shared" si="17"/>
+        <v>3399782.8225000012</v>
+      </c>
+      <c r="U199">
+        <f t="shared" si="18"/>
+        <v>77313859.408900037</v>
+      </c>
+      <c r="Z199">
+        <f t="shared" si="19"/>
+        <v>4654029798.2025013</v>
+      </c>
+      <c r="AE199">
+        <f t="shared" si="20"/>
+        <v>22024391294.068878</v>
+      </c>
+    </row>
+    <row r="200" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A200">
+        <f t="shared" si="14"/>
+        <v>1239.0399999999993</v>
+      </c>
+      <c r="F200">
+        <f t="shared" si="15"/>
+        <v>125.88840000000062</v>
+      </c>
+      <c r="K200">
+        <f t="shared" si="16"/>
+        <v>167370.99210000009</v>
+      </c>
+      <c r="P200">
+        <f t="shared" si="17"/>
+        <v>6714058.3224999979</v>
+      </c>
+      <c r="U200">
+        <f t="shared" si="18"/>
+        <v>59441478.628900029</v>
+      </c>
+      <c r="Z200">
+        <f t="shared" si="19"/>
+        <v>2170576851.3025012</v>
+      </c>
+      <c r="AE200">
+        <f t="shared" si="20"/>
+        <v>129145237238.90895</v>
+      </c>
+    </row>
+    <row r="201" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A201">
+        <f t="shared" si="14"/>
+        <v>1075.8400000000008</v>
+      </c>
+      <c r="F201">
+        <f t="shared" si="15"/>
+        <v>39291.16840000001</v>
+      </c>
+      <c r="K201">
+        <f t="shared" si="16"/>
+        <v>245906.89209999988</v>
+      </c>
+      <c r="P201">
+        <f t="shared" si="17"/>
+        <v>5708037.7224999983</v>
+      </c>
+      <c r="U201">
+        <f t="shared" si="18"/>
+        <v>13211989.128900012</v>
+      </c>
+      <c r="Z201">
+        <f t="shared" si="19"/>
+        <v>1674082231.8024991</v>
+      </c>
+      <c r="AE201">
+        <f t="shared" si="20"/>
+        <v>2026275500.7888932</v>
+      </c>
+    </row>
+    <row r="202" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A202">
+        <f t="shared" si="14"/>
+        <v>125.43999999999974</v>
+      </c>
+      <c r="F202">
+        <f t="shared" si="15"/>
+        <v>2095.8083999999976</v>
+      </c>
+      <c r="K202">
+        <f t="shared" si="16"/>
+        <v>4776.1921000000175</v>
+      </c>
+      <c r="P202">
+        <f t="shared" si="17"/>
+        <v>101219.42249999977</v>
+      </c>
+      <c r="U202">
+        <f t="shared" si="18"/>
+        <v>284670120.50889993</v>
+      </c>
+      <c r="Z202">
+        <f t="shared" si="19"/>
+        <v>3368125063.8024988</v>
+      </c>
+      <c r="AE202">
+        <f t="shared" si="20"/>
+        <v>8827322171.6689148</v>
+      </c>
+    </row>
+    <row r="203" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A203">
+        <f t="shared" si="14"/>
+        <v>77.440000000000197</v>
+      </c>
+      <c r="F203">
+        <f t="shared" si="15"/>
+        <v>26968.20840000001</v>
+      </c>
+      <c r="K203">
+        <f t="shared" si="16"/>
+        <v>194383.99209999989</v>
+      </c>
+      <c r="P203">
+        <f t="shared" si="17"/>
+        <v>749696.22250000061</v>
+      </c>
+      <c r="U203">
+        <f t="shared" si="18"/>
+        <v>916686434.84890008</v>
+      </c>
+      <c r="Z203">
+        <f t="shared" si="19"/>
+        <v>1573347923.7025008</v>
+      </c>
+      <c r="AE203">
+        <f t="shared" si="20"/>
+        <v>37125131530.16893</v>
+      </c>
+    </row>
+    <row r="204" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A204">
+        <f t="shared" si="14"/>
+        <v>392.04000000000048</v>
+      </c>
+      <c r="F204">
+        <f t="shared" si="15"/>
+        <v>77.088399999999524</v>
+      </c>
+      <c r="K204">
+        <f t="shared" si="16"/>
+        <v>15848.292099999968</v>
+      </c>
+      <c r="P204">
+        <f t="shared" si="17"/>
+        <v>5564173.3225000016</v>
+      </c>
+      <c r="U204">
+        <f t="shared" si="18"/>
+        <v>146914519.88890004</v>
+      </c>
+      <c r="Z204">
+        <f t="shared" si="19"/>
+        <v>197836883.70250031</v>
+      </c>
+      <c r="AE204">
+        <f t="shared" si="20"/>
+        <v>8018097491.0689135</v>
+      </c>
+    </row>
+    <row r="206" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A206">
+        <f>SQRT(AVERAGE(A105:A204))</f>
+        <v>29.274903928108795</v>
+      </c>
+      <c r="F206">
+        <f>SQRT(AVERAGE(F105:F204))</f>
+        <v>120.4598339696681</v>
+      </c>
+      <c r="K206">
+        <f>SQRT(AVERAGE(K105:K204))</f>
+        <v>484.38517514473955</v>
+      </c>
+      <c r="P206">
+        <f>SQRT(AVERAGE(P105:P204))</f>
+        <v>1968.898257274865</v>
+      </c>
+      <c r="U206">
+        <f>SQRT(AVERAGE(U105:U204))</f>
+        <v>12886.471708776611</v>
+      </c>
+      <c r="Z206">
+        <f>SQRT(AVERAGE(Z105:Z204))</f>
+        <v>42976.143837337237</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>